<commit_message>
Codigo de envio de gmail completo, faltan algunas validaciones extras
</commit_message>
<xml_diff>
--- a/importaciones/planilla-importacion.xlsx
+++ b/importaciones/planilla-importacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\boletas-pagos\importaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D205A264-D55C-459C-AA76-39DE3CBFB3C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66425603-AFF1-4E83-9761-87FE88DF5BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{76080FFF-C824-458A-AA84-29C7D7F3C4DF}"/>
   </bookViews>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04B1024-06D0-496C-8BE2-9D6EDE1ABA6A}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AV6" sqref="AV6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>